<commit_message>
Clinic Admin - Verify medical report
</commit_message>
<xml_diff>
--- a/src/test/resources/ClinicAdmin_TestData/Watts Health Center/Patient-details.xlsx
+++ b/src/test/resources/ClinicAdmin_TestData/Watts Health Center/Patient-details.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="PersonalDetails" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="61">
   <si>
     <t>Patient_ID</t>
   </si>
@@ -183,6 +183,25 @@
   </si>
   <si>
     <t>Followup comment and fee-1000</t>
+  </si>
+  <si>
+    <t>JPG-5MB.jpg</t>
+  </si>
+  <si>
+    <t>Oct 10, 2020</t>
+  </si>
+  <si>
+    <t>Report_name</t>
+  </si>
+  <si>
+    <t>Report_description</t>
+  </si>
+  <si>
+    <t>test,                             12,                              excel</t>
+  </si>
+  <si>
+    <t>JPG-1MB.jpg,                                       JPG-5MB.jpg, 
+New Microsoft Excel Worksheet.xlsx</t>
   </si>
 </sst>
 </file>
@@ -220,7 +239,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -243,11 +262,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -256,6 +286,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -640,7 +674,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -1088,10 +1122,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1100,9 +1134,11 @@
     <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.5703125" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
@@ -1115,106 +1151,140 @@
       <c r="D1" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>30</v>
       </c>
       <c r="D2" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="2">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>1</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>1</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="2">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>5</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="2">
-        <v>70</v>
+        <v>13</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A6:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>1</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>1</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>5</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>5</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>1</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Clinic Admin-Medical report, Patient-Batch file
</commit_message>
<xml_diff>
--- a/src/test/resources/ClinicAdmin_TestData/Watts Health Center/Patient-details.xlsx
+++ b/src/test/resources/ClinicAdmin_TestData/Watts Health Center/Patient-details.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="63">
   <si>
     <t>Patient_ID</t>
   </si>
@@ -195,13 +195,19 @@
   </si>
   <si>
     <t>Report_description</t>
-  </si>
-  <si>
-    <t>test,                             12,                              excel</t>
   </si>
   <si>
     <t>JPG-1MB.jpg,                                       JPG-5MB.jpg, 
 New Microsoft Excel Worksheet.xlsx</t>
+  </si>
+  <si>
+    <t>Oct 10, 2020 10:00 AM</t>
+  </si>
+  <si>
+    <t>No Documents uploaded</t>
+  </si>
+  <si>
+    <t>test,                                                  12,                                                    excel</t>
   </si>
 </sst>
 </file>
@@ -794,10 +800,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -907,16 +913,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>30</v>
       </c>
       <c r="D3" s="2">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>31</v>
@@ -934,33 +940,31 @@
         <v>36</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>54</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="L3" s="2"/>
       <c r="M3" s="2">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>30</v>
       </c>
       <c r="D4" s="2">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>31</v>
@@ -978,7 +982,7 @@
         <v>36</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="L4" s="2"/>
       <c r="M4" s="2">
@@ -993,16 +997,16 @@
         <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>30</v>
       </c>
       <c r="D5" s="2">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>31</v>
@@ -1020,34 +1024,36 @@
         <v>36</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L5" s="2"/>
+        <v>53</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="M5" s="2">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>30</v>
       </c>
       <c r="D6" s="2">
-        <v>70</v>
+        <v>1</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>32</v>
@@ -1056,13 +1062,13 @@
         <v>33</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>36</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="L6" s="2"/>
       <c r="M6" s="2">
@@ -1111,6 +1117,48 @@
         <v>2000</v>
       </c>
       <c r="N7" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="2">
+        <v>70</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2">
+        <v>2000</v>
+      </c>
+      <c r="N8" s="2" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1122,10 +1170,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A4" sqref="A4:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1135,7 +1183,7 @@
     <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28.5703125" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1158,24 +1206,44 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>30</v>
       </c>
       <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="2">
         <v>13</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="F2" s="6" t="s">
+      <c r="E3" s="4" t="s">
         <v>59</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1186,54 +1254,52 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A6:F12"/>
+  <dimension ref="A7:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>1</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="2">
-        <v>38</v>
-      </c>
-    </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>1</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>30</v>
       </c>
       <c r="D7" s="2">
-        <v>1</v>
+        <v>38</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>30</v>
       </c>
       <c r="D8" s="2">
-        <v>5</v>
+        <v>70</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1249,39 +1315,11 @@
       <c r="D9" s="2">
         <v>70</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>5</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="2">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <v>1</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="2">
-        <v>1</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>21</v>
+      <c r="E9" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>